<commit_message>
Messed around with the spreadsheets
</commit_message>
<xml_diff>
--- a/Virtual Machines/Results.xlsx
+++ b/Virtual Machines/Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="17">
   <si>
     <t>ackermann</t>
   </si>
@@ -80,6 +80,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -153,556 +154,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFC5000B"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFB3B3B3"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFD320"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF004586"/>
-      <rgbColor rgb="FF579D1C"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$54</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>C</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:dLbls>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$E$53:$K$53</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>ackermann</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>fasta</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>reversecomplement</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>mersenne</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>fannkuch</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>primesieve</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>mandelbrot</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$E$54:$K$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.193320894342367</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.355904783914953</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.504444722674346</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.401152715679422</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.913007062854725</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.337770006099044</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$56</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Normal</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="c5000b"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:dLbls>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$E$53:$K$53</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>ackermann</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>fasta</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>reversecomplement</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>mersenne</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>fannkuch</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>primesieve</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>mandelbrot</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$E$56:$K$56</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.41015410084708</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.44793017298631</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.45375548879131</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.2858394891699</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.34955815756972</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.09174081247973</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.48738555478387</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$57</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Table Only</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ffd320"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:dLbls>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$E$53:$K$53</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>ackermann</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>fasta</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>reversecomplement</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>mersenne</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>fannkuch</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>primesieve</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>mandelbrot</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$E$57:$K$57</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.29298987365614</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.25328104740521</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.13686156690548</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.09465381244522</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.18875240548019</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.0435406872801</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.29940525504934</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$55</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>register mapped</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="579d1c"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:dLbls>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$E$53:$K$53</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>ackermann</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>fasta</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>reversecomplement</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>mersenne</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>fannkuch</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>primesieve</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>mandelbrot</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$E$55:$K$55</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.29685602549678</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.10546788526612</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.05347816038826</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.11506197571053</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.06053672127067</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.951711437385443</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.875439184067745</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:gapWidth val="100"/>
-        <c:overlap val="0"/>
-        <c:axId val="78073316"/>
-        <c:axId val="7926699"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="78073316"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="7926699"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="7926699"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="78073316"/>
-        <c:crosses val="autoZero"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>672480</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>105120</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>431640</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>105120</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame>
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name=""/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="4736160" y="6282360"/>
-        <a:ext cx="7887240" cy="4064040"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -710,10 +162,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M57"/>
+  <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P38" activeCellId="0" sqref="P38"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L58" activeCellId="0" sqref="L58:L61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1955,10 +1407,6 @@
       <c r="D47" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="E47" s="0" t="n">
-        <f aca="false">L2</f>
-        <v>0</v>
-      </c>
       <c r="F47" s="0" t="n">
         <f aca="false">L8</f>
         <v>6.113</v>
@@ -2084,158 +1532,236 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E53" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="F53" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="G53" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="H53" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="I53" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="J53" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="K53" s="0" t="s">
-        <v>12</v>
+      <c r="D53" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" s="0" t="n">
+        <v>6.113</v>
+      </c>
+      <c r="G53" s="0" t="n">
+        <v>1.925</v>
+      </c>
+      <c r="H53" s="0" t="n">
+        <v>12.087</v>
+      </c>
+      <c r="I53" s="0" t="n">
+        <v>10.475</v>
+      </c>
+      <c r="J53" s="0" t="n">
+        <v>131.628</v>
+      </c>
+      <c r="K53" s="0" t="n">
+        <v>119.761</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D54" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E54" s="0" t="n">
-        <f aca="false">E47/AVERAGE(E$47:E$50)</f>
-        <v>0</v>
+        <v>142.25</v>
       </c>
       <c r="F54" s="0" t="n">
-        <f aca="false">F47/AVERAGE(F$47:F$50)</f>
-        <v>0.193320894342367</v>
+        <v>45.785</v>
       </c>
       <c r="G54" s="0" t="n">
-        <f aca="false">G47/AVERAGE(G$47:G$50)</f>
-        <v>0.355904783914953</v>
+        <v>7.863</v>
       </c>
       <c r="H54" s="0" t="n">
-        <f aca="false">H47/AVERAGE(H$47:H$50)</f>
-        <v>0.504444722674346</v>
+        <v>30.81</v>
       </c>
       <c r="I54" s="0" t="n">
-        <f aca="false">I47/AVERAGE(I$47:I$50)</f>
-        <v>0.401152715679422</v>
+        <v>35.24</v>
       </c>
       <c r="J54" s="0" t="n">
-        <f aca="false">J47/AVERAGE(J$47:J$50)</f>
-        <v>0.913007062854725</v>
+        <v>157.396</v>
       </c>
       <c r="K54" s="0" t="n">
-        <f aca="false">K47/AVERAGE(K$47:K$50)</f>
-        <v>0.337770006099044</v>
+        <v>527.373</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D55" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E55" s="0" t="n">
-        <f aca="false">E48/AVERAGE(E$47:E$50)</f>
-        <v>1.29685602549678</v>
+        <v>130.431</v>
       </c>
       <c r="F55" s="0" t="n">
-        <f aca="false">F48/AVERAGE(F$47:F$50)</f>
-        <v>1.10546788526612</v>
+        <v>39.63</v>
       </c>
       <c r="G55" s="0" t="n">
-        <f aca="false">G48/AVERAGE(G$47:G$50)</f>
-        <v>1.05347816038826</v>
+        <v>6.149</v>
       </c>
       <c r="H55" s="0" t="n">
-        <f aca="false">H48/AVERAGE(H$47:H$50)</f>
-        <v>1.11506197571053</v>
+        <v>26.229</v>
       </c>
       <c r="I55" s="0" t="n">
-        <f aca="false">I48/AVERAGE(I$47:I$50)</f>
-        <v>1.06053672127067</v>
+        <v>31.041</v>
       </c>
       <c r="J55" s="0" t="n">
-        <f aca="false">J48/AVERAGE(J$47:J$50)</f>
-        <v>0.951711437385443</v>
+        <v>150.447</v>
       </c>
       <c r="K55" s="0" t="n">
-        <f aca="false">K48/AVERAGE(K$47:K$50)</f>
-        <v>0.875439184067745</v>
+        <v>460.722</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D56" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E56" s="0" t="n">
+        <v>130.821</v>
+      </c>
+      <c r="F56" s="0" t="n">
+        <v>34.956</v>
+      </c>
+      <c r="G56" s="0" t="n">
+        <v>5.698</v>
+      </c>
+      <c r="H56" s="0" t="n">
+        <v>26.718</v>
+      </c>
+      <c r="I56" s="0" t="n">
+        <v>27.693</v>
+      </c>
+      <c r="J56" s="0" t="n">
+        <v>137.208</v>
+      </c>
+      <c r="K56" s="0" t="n">
+        <v>310.399</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D58" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F58" s="0" t="n">
+        <f aca="false">F53/F$53</f>
+        <v>1</v>
+      </c>
+      <c r="G58" s="0" t="n">
+        <f aca="false">G53/G$53</f>
+        <v>1</v>
+      </c>
+      <c r="H58" s="0" t="n">
+        <f aca="false">H53/H$53</f>
+        <v>1</v>
+      </c>
+      <c r="I58" s="0" t="n">
+        <f aca="false">I53/I$53</f>
+        <v>1</v>
+      </c>
+      <c r="J58" s="0" t="n">
+        <f aca="false">J53/J$53</f>
+        <v>1</v>
+      </c>
+      <c r="K58" s="0" t="n">
+        <f aca="false">K53/K$53</f>
+        <v>1</v>
+      </c>
+      <c r="L58" s="0" t="n">
+        <f aca="false">AVERAGE(F58:K58)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D59" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E56" s="0" t="n">
-        <f aca="false">E49/AVERAGE(E$47:E$50)</f>
-        <v>1.41015410084708</v>
-      </c>
-      <c r="F56" s="0" t="n">
-        <f aca="false">F49/AVERAGE(F$47:F$50)</f>
-        <v>1.44793017298631</v>
-      </c>
-      <c r="G56" s="0" t="n">
-        <f aca="false">G49/AVERAGE(G$47:G$50)</f>
-        <v>1.45375548879131</v>
-      </c>
-      <c r="H56" s="0" t="n">
-        <f aca="false">H49/AVERAGE(H$47:H$50)</f>
-        <v>1.2858394891699</v>
-      </c>
-      <c r="I56" s="0" t="n">
-        <f aca="false">I49/AVERAGE(I$47:I$50)</f>
-        <v>1.34955815756972</v>
-      </c>
-      <c r="J56" s="0" t="n">
-        <f aca="false">J49/AVERAGE(J$47:J$50)</f>
-        <v>1.09174081247973</v>
-      </c>
-      <c r="K56" s="0" t="n">
-        <f aca="false">K49/AVERAGE(K$47:K$50)</f>
-        <v>1.48738555478387</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D57" s="0" t="s">
+      <c r="F59" s="0" t="n">
+        <f aca="false">F54/F$53</f>
+        <v>7.48977588745297</v>
+      </c>
+      <c r="G59" s="0" t="n">
+        <f aca="false">G54/G$53</f>
+        <v>4.08467532467533</v>
+      </c>
+      <c r="H59" s="0" t="n">
+        <f aca="false">H54/H$53</f>
+        <v>2.54901960784314</v>
+      </c>
+      <c r="I59" s="0" t="n">
+        <f aca="false">I54/I$53</f>
+        <v>3.36420047732697</v>
+      </c>
+      <c r="J59" s="0" t="n">
+        <f aca="false">J54/J$53</f>
+        <v>1.19576381924818</v>
+      </c>
+      <c r="K59" s="0" t="n">
+        <f aca="false">K54/K$53</f>
+        <v>4.40354539457753</v>
+      </c>
+      <c r="L59" s="0" t="n">
+        <f aca="false">AVERAGE(F59:K59)</f>
+        <v>3.84783008518735</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D60" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E57" s="0" t="n">
-        <f aca="false">E50/AVERAGE(E$47:E$50)</f>
-        <v>1.29298987365614</v>
-      </c>
-      <c r="F57" s="0" t="n">
-        <f aca="false">F50/AVERAGE(F$47:F$50)</f>
-        <v>1.25328104740521</v>
-      </c>
-      <c r="G57" s="0" t="n">
-        <f aca="false">G50/AVERAGE(G$47:G$50)</f>
-        <v>1.13686156690548</v>
-      </c>
-      <c r="H57" s="0" t="n">
-        <f aca="false">H50/AVERAGE(H$47:H$50)</f>
-        <v>1.09465381244522</v>
-      </c>
-      <c r="I57" s="0" t="n">
-        <f aca="false">I50/AVERAGE(I$47:I$50)</f>
-        <v>1.18875240548019</v>
-      </c>
-      <c r="J57" s="0" t="n">
-        <f aca="false">J50/AVERAGE(J$47:J$50)</f>
-        <v>1.0435406872801</v>
-      </c>
-      <c r="K57" s="0" t="n">
-        <f aca="false">K50/AVERAGE(K$47:K$50)</f>
-        <v>1.29940525504934</v>
+      <c r="F60" s="0" t="n">
+        <f aca="false">F55/F$53</f>
+        <v>6.48290528382136</v>
+      </c>
+      <c r="G60" s="0" t="n">
+        <f aca="false">G55/G$53</f>
+        <v>3.19428571428571</v>
+      </c>
+      <c r="H60" s="0" t="n">
+        <f aca="false">H55/H$53</f>
+        <v>2.17001737403822</v>
+      </c>
+      <c r="I60" s="0" t="n">
+        <f aca="false">I55/I$53</f>
+        <v>2.96334128878282</v>
+      </c>
+      <c r="J60" s="0" t="n">
+        <f aca="false">J55/J$53</f>
+        <v>1.14297110037378</v>
+      </c>
+      <c r="K60" s="0" t="n">
+        <f aca="false">K55/K$53</f>
+        <v>3.84701196549795</v>
+      </c>
+      <c r="L60" s="0" t="n">
+        <f aca="false">AVERAGE(F60:K60)</f>
+        <v>3.30008878779998</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D61" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F61" s="0" t="n">
+        <f aca="false">F56/F$53</f>
+        <v>5.7183052511042</v>
+      </c>
+      <c r="G61" s="0" t="n">
+        <f aca="false">G56/G$53</f>
+        <v>2.96</v>
+      </c>
+      <c r="H61" s="0" t="n">
+        <f aca="false">H56/H$53</f>
+        <v>2.21047406304294</v>
+      </c>
+      <c r="I61" s="0" t="n">
+        <f aca="false">I56/I$53</f>
+        <v>2.643723150358</v>
+      </c>
+      <c r="J61" s="0" t="n">
+        <f aca="false">J56/J$53</f>
+        <v>1.04239219618926</v>
+      </c>
+      <c r="K61" s="0" t="n">
+        <f aca="false">K56/K$53</f>
+        <v>2.59182037558137</v>
+      </c>
+      <c r="L61" s="0" t="n">
+        <f aca="false">AVERAGE(F61:K61)</f>
+        <v>2.86111917271263</v>
       </c>
     </row>
   </sheetData>
@@ -2246,6 +1772,5 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>